<commit_message>
feat: complete Excel impl
</commit_message>
<xml_diff>
--- a/backend/resources/grade-offline-template.xlsx
+++ b/backend/resources/grade-offline-template.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neo/Desktop/NYU/2024/Software Engineering/Darkspace/backend/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336F8EDB-02FE-5447-A304-D21BB51332A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC28FCC-8122-624B-BCE5-AC3560539E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12360" yWindow="30500" windowWidth="21900" windowHeight="19680" xr2:uid="{2A01D6A5-069E-B74D-8D99-99C0557690D7}"/>
+    <workbookView xWindow="9300" yWindow="30120" windowWidth="25580" windowHeight="19680" xr2:uid="{2A01D6A5-069E-B74D-8D99-99C0557690D7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="submissions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Feedback</t>
+  </si>
+  <si>
+    <t>Course ID</t>
+  </si>
+  <si>
+    <t>Assignment ID</t>
   </si>
 </sst>
 </file>
@@ -66,7 +72,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +106,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -116,13 +128,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84E0ED0-257E-8C4E-8F09-482EE4CABCB6}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,9 +463,11 @@
     <col min="3" max="3" width="7.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -467,6 +482,12 @@
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>